<commit_message>
Create automatic decoder script
</commit_message>
<xml_diff>
--- a/GR_timestamps.xlsx
+++ b/GR_timestamps.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="12160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="12160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
+    <sheet name="גיליון2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -138,6 +139,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -148,18 +161,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -975,7 +976,857 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="he-IL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="#,##0.0000000000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>גיליון2!$D$2:$D$79</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="78"/>
+                <c:pt idx="0">
+                  <c:v>-77</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-77</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-78</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-79</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-79</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-81</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-82</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-81</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-83</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-84</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-85</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-84</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-84</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-85</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-85</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-86</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-86</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-86</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-82</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-89</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-89</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-89</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-90</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-93</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-92</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-92</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-92</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-92</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-92</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-92</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-92</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-93</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-93</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-93</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-93</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-93</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-94</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-93</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-94</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-95</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-94</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-95</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-95</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-96</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-95</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-95</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-96</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-96</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-96</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-97</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-97</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-97</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-97</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-98</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-99</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-99</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-99</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-100</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-99</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-99</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-100</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-100</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-100</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-100</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-101</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-101</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-101</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-102</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-102</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-102</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-103</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-104</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-104</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-103</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-106</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-106</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-105</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>גיליון2!$E$2:$E$79</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="78"/>
+                <c:pt idx="0">
+                  <c:v>39392</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39396</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39398</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39404</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39404</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39398</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39400</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39402</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39407</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>39406</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39408</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39410</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39408</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39406</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>39408</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39406</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>39402</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39413</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>39414</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>39414</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>39418</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>39418</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>39417</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>39417</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>39417</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>39420</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>39418</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>39416</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>39418</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>39421</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>39421</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>39420</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>39420</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>39420</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0">
+                  <c:v>39420</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0">
+                  <c:v>39419</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="0">
+                  <c:v>39419</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="0">
+                  <c:v>39422</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="0">
+                  <c:v>39422</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="0">
+                  <c:v>39422</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="0">
+                  <c:v>39422</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="0">
+                  <c:v>39424</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="0">
+                  <c:v>39420</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="0">
+                  <c:v>39422</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="0">
+                  <c:v>39424</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="0">
+                  <c:v>39424</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="0">
+                  <c:v>39425</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="0">
+                  <c:v>39426</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="0">
+                  <c:v>39426</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="0">
+                  <c:v>39426</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="0">
+                  <c:v>39427</c:v>
+                </c:pt>
+                <c:pt idx="53" formatCode="0">
+                  <c:v>39427</c:v>
+                </c:pt>
+                <c:pt idx="54" formatCode="0">
+                  <c:v>39430</c:v>
+                </c:pt>
+                <c:pt idx="55" formatCode="0">
+                  <c:v>39430</c:v>
+                </c:pt>
+                <c:pt idx="56" formatCode="0">
+                  <c:v>39429</c:v>
+                </c:pt>
+                <c:pt idx="57" formatCode="0">
+                  <c:v>39430</c:v>
+                </c:pt>
+                <c:pt idx="58" formatCode="0">
+                  <c:v>39430</c:v>
+                </c:pt>
+                <c:pt idx="59" formatCode="0">
+                  <c:v>39431</c:v>
+                </c:pt>
+                <c:pt idx="60" formatCode="0">
+                  <c:v>39432</c:v>
+                </c:pt>
+                <c:pt idx="61" formatCode="0">
+                  <c:v>39431</c:v>
+                </c:pt>
+                <c:pt idx="62" formatCode="0">
+                  <c:v>39431</c:v>
+                </c:pt>
+                <c:pt idx="63" formatCode="0">
+                  <c:v>39431</c:v>
+                </c:pt>
+                <c:pt idx="64" formatCode="0">
+                  <c:v>39432</c:v>
+                </c:pt>
+                <c:pt idx="65" formatCode="0">
+                  <c:v>39433</c:v>
+                </c:pt>
+                <c:pt idx="66" formatCode="0">
+                  <c:v>39434</c:v>
+                </c:pt>
+                <c:pt idx="67" formatCode="0">
+                  <c:v>39436</c:v>
+                </c:pt>
+                <c:pt idx="68" formatCode="0">
+                  <c:v>39436</c:v>
+                </c:pt>
+                <c:pt idx="69" formatCode="0">
+                  <c:v>39437</c:v>
+                </c:pt>
+                <c:pt idx="70" formatCode="0">
+                  <c:v>39439</c:v>
+                </c:pt>
+                <c:pt idx="71" formatCode="0">
+                  <c:v>39439</c:v>
+                </c:pt>
+                <c:pt idx="72" formatCode="0">
+                  <c:v>39439</c:v>
+                </c:pt>
+                <c:pt idx="73" formatCode="0">
+                  <c:v>39440</c:v>
+                </c:pt>
+                <c:pt idx="74" formatCode="0">
+                  <c:v>39442</c:v>
+                </c:pt>
+                <c:pt idx="75" formatCode="0">
+                  <c:v>39444</c:v>
+                </c:pt>
+                <c:pt idx="76" formatCode="0">
+                  <c:v>39444</c:v>
+                </c:pt>
+                <c:pt idx="77" formatCode="0">
+                  <c:v>39444</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DB45-43FD-A940-279F65417BFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="254567647"/>
+        <c:axId val="16558031"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="254567647"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="16558031"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="16558031"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="254567647"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1531,6 +2382,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1550,6 +2917,43 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="תרשים 2"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>75754</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>129250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>415094</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>180524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="תרשים 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1831,8 +3235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1845,14 +3249,14 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -1864,7 +3268,7 @@
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1882,10 +3286,10 @@
         <f>C4-4</f>
         <v>39392</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="4">
         <v>34.060548601662802</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="4">
         <v>39387</v>
       </c>
     </row>
@@ -1900,10 +3304,10 @@
         <f>C5-2</f>
         <v>39396</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="4">
         <v>45.795238095237998</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="4">
         <v>39390</v>
       </c>
     </row>
@@ -1914,13 +3318,13 @@
       <c r="B5" s="3">
         <v>55.666666666666899</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="4">
         <v>39398</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="4">
         <v>56.924943310657902</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="4">
         <v>39392</v>
       </c>
     </row>
@@ -1935,10 +3339,10 @@
         <f>C5+2</f>
         <v>39400</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="4">
         <v>68.881179142086395</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="4">
         <v>39394</v>
       </c>
     </row>
@@ -1953,10 +3357,10 @@
         <f>C6</f>
         <v>39400</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>80.533560092902306</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="4">
         <v>39392</v>
       </c>
     </row>
@@ -1971,10 +3375,10 @@
         <f>C7+4</f>
         <v>39404</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="4">
         <v>91.997732424580505</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="4">
         <v>39394</v>
       </c>
     </row>
@@ -1989,10 +3393,10 @@
         <f>C8</f>
         <v>39404</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="4">
         <v>103.160770973333</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="4">
         <v>39396</v>
       </c>
     </row>
@@ -2007,10 +3411,10 @@
         <f>C9-6</f>
         <v>39398</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="4">
         <v>114.314058955193</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="4">
         <v>39398</v>
       </c>
     </row>
@@ -2025,10 +3429,10 @@
         <f>C10+2</f>
         <v>39400</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="4">
         <v>125.78049886449</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="4">
         <v>39400</v>
       </c>
     </row>
@@ -2043,10 +3447,10 @@
         <f>C11+2</f>
         <v>39402</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="4">
         <v>137.06446383582701</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="4">
         <v>39402</v>
       </c>
     </row>
@@ -2061,10 +3465,10 @@
         <f>C12+5</f>
         <v>39407</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="4">
         <v>149.09276802403599</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="4">
         <v>39404</v>
       </c>
     </row>
@@ -2079,10 +3483,10 @@
         <f>C13-1</f>
         <v>39406</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="4">
         <v>160.385690081631</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="4">
         <v>39402</v>
       </c>
     </row>
@@ -2097,10 +3501,10 @@
         <f>C14+2</f>
         <v>39408</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="4">
         <v>172.47852272606801</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="4">
         <v>39404</v>
       </c>
     </row>
@@ -2115,10 +3519,10 @@
         <f>C15+2</f>
         <v>39410</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="4">
         <v>183.48169897868399</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="4">
         <v>39406</v>
       </c>
     </row>
@@ -2133,10 +3537,10 @@
         <f>C16-2</f>
         <v>39408</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="4">
         <v>194.93962096417101</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="4">
         <v>39404</v>
       </c>
     </row>
@@ -2151,10 +3555,10 @@
         <f>C17-2</f>
         <v>39406</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="4">
         <v>206.219084854421</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="4">
         <v>39406</v>
       </c>
     </row>
@@ -2169,10 +3573,10 @@
         <f>C18+2</f>
         <v>39408</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="4">
         <v>217.81591025124601</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="4">
         <v>39406</v>
       </c>
     </row>
@@ -2187,10 +3591,10 @@
         <f>C19-2</f>
         <v>39406</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="4">
         <v>229.186885307936</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="4">
         <v>39404</v>
       </c>
     </row>
@@ -2205,10 +3609,10 @@
         <f>C20-4</f>
         <v>39402</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="4">
         <v>240.76693065941001</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="4">
         <v>39398</v>
       </c>
     </row>
@@ -2223,10 +3627,10 @@
         <f>C21+11</f>
         <v>39413</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="4">
         <v>252.378041770522</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="4">
         <v>39411</v>
       </c>
     </row>
@@ -2241,10 +3645,10 @@
         <f>C22+1</f>
         <v>39414</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="4">
         <v>263.85219143038597</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="4">
         <v>39411</v>
       </c>
     </row>
@@ -2259,10 +3663,10 @@
         <f>C23</f>
         <v>39414</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="4">
         <v>275.191193697958</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="4">
         <v>39413</v>
       </c>
     </row>
@@ -2277,10 +3681,10 @@
         <f>C24+4</f>
         <v>39418</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="4">
         <v>286.803892110655</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="4">
         <v>39414</v>
       </c>
     </row>
@@ -2295,10 +3699,10 @@
         <f>C25</f>
         <v>39418</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="4">
         <v>298.48597827845498</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="4">
         <v>39418</v>
       </c>
     </row>
@@ -2313,10 +3717,10 @@
         <f>C26-1</f>
         <v>39417</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="4">
         <v>309.97237283627902</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="4">
         <v>39416</v>
       </c>
     </row>
@@ -2331,10 +3735,10 @@
         <f>C27</f>
         <v>39417</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="4">
         <v>321.61092158911299</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="4">
         <v>39416</v>
       </c>
     </row>
@@ -2349,10 +3753,10 @@
         <f>C28</f>
         <v>39417</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="4">
         <v>333.31772431020198</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="4">
         <f>E28</f>
         <v>39416</v>
       </c>
@@ -2368,10 +3772,10 @@
         <f>C29+3</f>
         <v>39420</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="4">
         <v>344.62747487709402</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="4">
         <v>39418</v>
       </c>
     </row>
@@ -2386,10 +3790,10 @@
         <f>C30-2</f>
         <v>39418</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="4">
         <v>355.93858598820498</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="4">
         <v>39418</v>
       </c>
     </row>
@@ -2404,10 +3808,10 @@
         <f>C31-2</f>
         <v>39416</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="4">
         <v>368.00865401541603</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="4">
         <v>39418</v>
       </c>
     </row>
@@ -2422,10 +3826,10 @@
         <f>C32+2</f>
         <v>39418</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="4">
         <v>379.36103496779702</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="4">
         <v>39420</v>
       </c>
     </row>
@@ -2440,10 +3844,10 @@
         <f>C33+3</f>
         <v>39421</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="4">
         <v>391.08212340317101</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="4">
         <v>39419</v>
       </c>
     </row>
@@ -2458,10 +3862,10 @@
         <f>C34</f>
         <v>39421</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="4">
         <v>402.55060412879402</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="4">
         <v>39419</v>
       </c>
     </row>
@@ -2476,10 +3880,10 @@
         <f>C35-1</f>
         <v>39420</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D36" s="4">
         <v>413.949243584577</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E36" s="4">
         <v>39419</v>
       </c>
     </row>
@@ -2494,10 +3898,10 @@
         <f>C36</f>
         <v>39420</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D37" s="4">
         <v>425.209334287525</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="4">
         <v>39419</v>
       </c>
     </row>
@@ -2512,10 +3916,10 @@
         <f>C37</f>
         <v>39420</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D38" s="4">
         <v>436.48371070475901</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="4">
         <v>39419</v>
       </c>
     </row>
@@ -2523,10 +3927,10 @@
       <c r="A39" s="3">
         <v>36</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B39" s="5">
         <v>448.81430011318503</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="6">
         <f>C38</f>
         <v>39420</v>
       </c>
@@ -2544,7 +3948,7 @@
       <c r="B40" s="3">
         <v>460.22724767460602</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="6">
         <f>C39-1</f>
         <v>39419</v>
       </c>
@@ -2562,7 +3966,7 @@
       <c r="B41" s="3">
         <v>472.62908412491697</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="6">
         <f>C40</f>
         <v>39419</v>
       </c>
@@ -2580,7 +3984,7 @@
       <c r="B42" s="3">
         <v>483.949302304887</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="6">
         <f>C41+3</f>
         <v>39422</v>
       </c>
@@ -2598,7 +4002,7 @@
       <c r="B43" s="3">
         <v>495.67955944060998</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="6">
         <f>C42</f>
         <v>39422</v>
       </c>
@@ -2616,7 +4020,7 @@
       <c r="B44" s="3">
         <v>507.30596170105099</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="6">
         <f>C43</f>
         <v>39422</v>
       </c>
@@ -2634,7 +4038,7 @@
       <c r="B45" s="3">
         <v>518.94506474447496</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="6">
         <f>C44</f>
         <v>39422</v>
       </c>
@@ -2653,7 +4057,7 @@
       <c r="B46" s="3">
         <v>530.70427235242903</v>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="6">
         <f>C45+2</f>
         <v>39424</v>
       </c>
@@ -2671,7 +4075,7 @@
       <c r="B47" s="3">
         <v>542.40384277217197</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="6">
         <f>C46-4</f>
         <v>39420</v>
       </c>
@@ -2689,7 +4093,7 @@
       <c r="B48" s="3">
         <v>554.16010253432103</v>
       </c>
-      <c r="C48" s="10">
+      <c r="C48" s="6">
         <f>C47+2</f>
         <v>39422</v>
       </c>
@@ -2707,7 +4111,7 @@
       <c r="B49" s="3">
         <v>565.93994506290801</v>
       </c>
-      <c r="C49" s="10">
+      <c r="C49" s="6">
         <f>C48+2</f>
         <v>39424</v>
       </c>
@@ -2725,7 +4129,7 @@
       <c r="B50" s="3">
         <v>577.03203248945499</v>
       </c>
-      <c r="C50" s="10">
+      <c r="C50" s="6">
         <f>C49</f>
         <v>39424</v>
       </c>
@@ -2743,7 +4147,7 @@
       <c r="B51" s="3">
         <v>588.51019263114097</v>
       </c>
-      <c r="C51" s="10">
+      <c r="C51" s="6">
         <f>C50+1</f>
         <v>39425</v>
       </c>
@@ -2761,7 +4165,7 @@
       <c r="B52" s="3">
         <v>600.11274731523497</v>
       </c>
-      <c r="C52" s="10">
+      <c r="C52" s="6">
         <f>C51+1</f>
         <v>39426</v>
       </c>
@@ -2779,7 +4183,7 @@
       <c r="B53" s="3">
         <v>611.84228612629704</v>
       </c>
-      <c r="C53" s="10">
+      <c r="C53" s="6">
         <f>C52</f>
         <v>39426</v>
       </c>
@@ -2797,7 +4201,7 @@
       <c r="B54" s="3">
         <v>623.64098593509698</v>
       </c>
-      <c r="C54" s="10">
+      <c r="C54" s="6">
         <f>C53</f>
         <v>39426</v>
       </c>
@@ -2815,7 +4219,7 @@
       <c r="B55" s="3">
         <v>634.805898895822</v>
       </c>
-      <c r="C55" s="10">
+      <c r="C55" s="6">
         <f>C54+1</f>
         <v>39427</v>
       </c>
@@ -2833,7 +4237,7 @@
       <c r="B56" s="3">
         <v>646.18192296765801</v>
       </c>
-      <c r="C56" s="10">
+      <c r="C56" s="6">
         <f>C55</f>
         <v>39427</v>
       </c>
@@ -2852,7 +4256,7 @@
       <c r="B57" s="3">
         <v>657.34683592837803</v>
       </c>
-      <c r="C57" s="10">
+      <c r="C57" s="6">
         <f>C56+3</f>
         <v>39430</v>
       </c>
@@ -2870,7 +4274,7 @@
       <c r="B58" s="3">
         <v>669.04825682561295</v>
       </c>
-      <c r="C58" s="10">
+      <c r="C58" s="6">
         <f>C57</f>
         <v>39430</v>
       </c>
@@ -2888,7 +4292,7 @@
       <c r="B59" s="3">
         <v>680.61385005844704</v>
       </c>
-      <c r="C59" s="10">
+      <c r="C59" s="6">
         <f>C58-1</f>
         <v>39429</v>
       </c>
@@ -2906,7 +4310,7 @@
       <c r="B60" s="3">
         <v>691.51391041146303</v>
       </c>
-      <c r="C60" s="10">
+      <c r="C60" s="6">
         <f>C59+1</f>
         <v>39430</v>
       </c>
@@ -2924,7 +4328,7 @@
       <c r="B61" s="3">
         <v>703.16000251051298</v>
       </c>
-      <c r="C61" s="10">
+      <c r="C61" s="6">
         <f>C60</f>
         <v>39430</v>
       </c>
@@ -2939,10 +4343,10 @@
       <c r="A62" s="3">
         <v>59</v>
       </c>
-      <c r="B62" s="8">
+      <c r="B62" s="4">
         <v>714.52940581315704</v>
       </c>
-      <c r="C62" s="11">
+      <c r="C62" s="7">
         <f>C61+1</f>
         <v>39431</v>
       </c>
@@ -2957,10 +4361,10 @@
       <c r="A63" s="3">
         <v>60</v>
       </c>
-      <c r="B63" s="8">
+      <c r="B63" s="4">
         <v>725.66310386181704</v>
       </c>
-      <c r="C63" s="11">
+      <c r="C63" s="7">
         <f>C62+1</f>
         <v>39432</v>
       </c>
@@ -2975,10 +4379,10 @@
       <c r="A64" s="3">
         <v>61</v>
       </c>
-      <c r="B64" s="8">
+      <c r="B64" s="4">
         <v>737.120157919549</v>
       </c>
-      <c r="C64" s="11">
+      <c r="C64" s="7">
         <f>C63-1</f>
         <v>39431</v>
       </c>
@@ -2993,10 +4397,10 @@
       <c r="A65" s="3">
         <v>62</v>
       </c>
-      <c r="B65" s="8">
+      <c r="B65" s="4">
         <v>748.17063601356199</v>
       </c>
-      <c r="C65" s="11">
+      <c r="C65" s="7">
         <f>C64</f>
         <v>39431</v>
       </c>
@@ -3011,10 +4415,10 @@
       <c r="A66" s="3">
         <v>63</v>
       </c>
-      <c r="B66" s="8">
+      <c r="B66" s="4">
         <v>759.83744063818699</v>
       </c>
-      <c r="C66" s="11">
+      <c r="C66" s="7">
         <f>C65</f>
         <v>39431</v>
       </c>
@@ -3029,10 +4433,10 @@
       <c r="A67" s="3">
         <v>64</v>
       </c>
-      <c r="B67" s="8">
+      <c r="B67" s="4">
         <v>771.24011026861797</v>
       </c>
-      <c r="C67" s="11">
+      <c r="C67" s="7">
         <f>C66+1</f>
         <v>39432</v>
       </c>
@@ -3047,10 +4451,10 @@
       <c r="A68" s="3">
         <v>65</v>
       </c>
-      <c r="B68" s="8">
+      <c r="B68" s="4">
         <v>782.96003456448898</v>
       </c>
-      <c r="C68" s="11">
+      <c r="C68" s="7">
         <f>C67+1</f>
         <v>39433</v>
       </c>
@@ -3065,10 +4469,10 @@
       <c r="A69" s="3">
         <v>66</v>
       </c>
-      <c r="B69" s="8">
+      <c r="B69" s="4">
         <v>794.12258924585103</v>
       </c>
-      <c r="C69" s="11">
+      <c r="C69" s="7">
         <f>C68+1</f>
         <v>39434</v>
       </c>
@@ -3083,10 +4487,10 @@
       <c r="A70" s="3">
         <v>67</v>
       </c>
-      <c r="B70" s="8">
+      <c r="B70" s="4">
         <v>805.96088088865804</v>
       </c>
-      <c r="C70" s="11">
+      <c r="C70" s="7">
         <f>C69+2</f>
         <v>39436</v>
       </c>
@@ -3101,10 +4505,10 @@
       <c r="A71" s="3">
         <v>68</v>
       </c>
-      <c r="B71" s="8">
+      <c r="B71" s="4">
         <v>816.95835620493801</v>
       </c>
-      <c r="C71" s="11">
+      <c r="C71" s="7">
         <f>C70</f>
         <v>39436</v>
       </c>
@@ -3119,10 +4523,10 @@
       <c r="A72" s="3">
         <v>69</v>
       </c>
-      <c r="B72" s="8">
+      <c r="B72" s="4">
         <v>828.871388565291</v>
       </c>
-      <c r="C72" s="11">
+      <c r="C72" s="7">
         <f>C71+1</f>
         <v>39437</v>
       </c>
@@ -3137,10 +4541,10 @@
       <c r="A73" s="3">
         <v>70</v>
       </c>
-      <c r="B73" s="8">
+      <c r="B73" s="4">
         <v>840.84677422583297</v>
       </c>
-      <c r="C73" s="11">
+      <c r="C73" s="7">
         <f>C72+2</f>
         <v>39439</v>
       </c>
@@ -3155,10 +4559,10 @@
       <c r="A74" s="3">
         <v>71</v>
       </c>
-      <c r="B74" s="8">
+      <c r="B74" s="4">
         <v>854.28882655304301</v>
       </c>
-      <c r="C74" s="11">
+      <c r="C74" s="7">
         <f>C73</f>
         <v>39439</v>
       </c>
@@ -3173,10 +4577,10 @@
       <c r="A75" s="3">
         <v>72</v>
       </c>
-      <c r="B75" s="8">
+      <c r="B75" s="4">
         <v>865.32589021812203</v>
       </c>
-      <c r="C75" s="11">
+      <c r="C75" s="7">
         <f>C74</f>
         <v>39439</v>
       </c>
@@ -3191,10 +4595,10 @@
       <c r="A76" s="3">
         <v>73</v>
       </c>
-      <c r="B76" s="8">
+      <c r="B76" s="4">
         <v>876.94640059521601</v>
       </c>
-      <c r="C76" s="11">
+      <c r="C76" s="7">
         <f>C75+1</f>
         <v>39440</v>
       </c>
@@ -3209,10 +4613,10 @@
       <c r="A77" s="3">
         <v>74</v>
       </c>
-      <c r="B77" s="8">
+      <c r="B77" s="4">
         <v>888.01158217412103</v>
       </c>
-      <c r="C77" s="11">
+      <c r="C77" s="7">
         <f>C76+2</f>
         <v>39442</v>
       </c>
@@ -3227,10 +4631,10 @@
       <c r="A78" s="3">
         <v>75</v>
       </c>
-      <c r="B78" s="8">
+      <c r="B78" s="4">
         <v>899.30646896844996</v>
       </c>
-      <c r="C78" s="11">
+      <c r="C78" s="7">
         <f>C77+2</f>
         <v>39444</v>
       </c>
@@ -3245,10 +4649,10 @@
       <c r="A79" s="3">
         <v>76</v>
       </c>
-      <c r="B79" s="8">
+      <c r="B79" s="4">
         <v>910.98230814373005</v>
       </c>
-      <c r="C79" s="11">
+      <c r="C79" s="7">
         <f>C78</f>
         <v>39444</v>
       </c>
@@ -3263,10 +4667,10 @@
       <c r="A80" s="3">
         <v>77</v>
       </c>
-      <c r="B80" s="8">
+      <c r="B80" s="4">
         <v>923.07265979066597</v>
       </c>
-      <c r="C80" s="11">
+      <c r="C80" s="7">
         <f>C79</f>
         <v>39444</v>
       </c>
@@ -3286,4 +4690,1816 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D2:I79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="135" zoomScaleNormal="161" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D2">
+        <v>-77</v>
+      </c>
+      <c r="E2" s="3">
+        <f>E3-4</f>
+        <v>39392</v>
+      </c>
+      <c r="F2">
+        <f>E2/44100</f>
+        <v>0.89324263038548757</v>
+      </c>
+      <c r="G2">
+        <v>-78</v>
+      </c>
+      <c r="H2" s="4">
+        <v>39387</v>
+      </c>
+      <c r="I2">
+        <f>H2/44100</f>
+        <v>0.89312925170068025</v>
+      </c>
+    </row>
+    <row r="3" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <v>-77</v>
+      </c>
+      <c r="E3" s="3">
+        <f>E4-2</f>
+        <v>39396</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F66" si="0">E3/44100</f>
+        <v>0.89333333333333331</v>
+      </c>
+      <c r="G3">
+        <v>-82</v>
+      </c>
+      <c r="H3" s="4">
+        <v>39390</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I66" si="1">H3/44100</f>
+        <v>0.89319727891156464</v>
+      </c>
+    </row>
+    <row r="4" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <v>-78</v>
+      </c>
+      <c r="E4" s="4">
+        <v>39398</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89337868480725624</v>
+      </c>
+      <c r="G4">
+        <v>-81</v>
+      </c>
+      <c r="H4" s="4">
+        <v>39392</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89324263038548757</v>
+      </c>
+    </row>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <v>-79</v>
+      </c>
+      <c r="E5" s="3">
+        <f>E4+2</f>
+        <v>39400</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89342403628117917</v>
+      </c>
+      <c r="G5">
+        <v>-82</v>
+      </c>
+      <c r="H5" s="4">
+        <v>39394</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89328798185941038</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <v>-79</v>
+      </c>
+      <c r="E6" s="3">
+        <f>E5</f>
+        <v>39400</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89342403628117917</v>
+      </c>
+      <c r="G6">
+        <v>-82</v>
+      </c>
+      <c r="H6" s="4">
+        <v>39392</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89324263038548757</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D7">
+        <v>-81</v>
+      </c>
+      <c r="E7" s="3">
+        <f>E6+4</f>
+        <v>39404</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89351473922902491</v>
+      </c>
+      <c r="G7">
+        <v>-85</v>
+      </c>
+      <c r="H7" s="4">
+        <v>39394</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89328798185941038</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <v>-82</v>
+      </c>
+      <c r="E8" s="3">
+        <f>E7</f>
+        <v>39404</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89351473922902491</v>
+      </c>
+      <c r="G8">
+        <v>-85</v>
+      </c>
+      <c r="H8" s="4">
+        <v>39396</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89333333333333331</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <v>-81</v>
+      </c>
+      <c r="E9" s="3">
+        <f>E8-6</f>
+        <v>39398</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89337868480725624</v>
+      </c>
+      <c r="G9">
+        <v>-81</v>
+      </c>
+      <c r="H9" s="4">
+        <v>39398</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89337868480725624</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <v>-83</v>
+      </c>
+      <c r="E10" s="3">
+        <f>E9+2</f>
+        <v>39400</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89342403628117917</v>
+      </c>
+      <c r="G10">
+        <v>-84</v>
+      </c>
+      <c r="H10" s="4">
+        <v>39400</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89342403628117917</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D11">
+        <v>-84</v>
+      </c>
+      <c r="E11" s="3">
+        <f>E10+2</f>
+        <v>39402</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8934693877551021</v>
+      </c>
+      <c r="G11">
+        <v>-84</v>
+      </c>
+      <c r="H11" s="4">
+        <v>39402</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.8934693877551021</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D12">
+        <v>-85</v>
+      </c>
+      <c r="E12" s="3">
+        <f>E11+5</f>
+        <v>39407</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8935827664399093</v>
+      </c>
+      <c r="G12">
+        <v>-87</v>
+      </c>
+      <c r="H12" s="4">
+        <v>39404</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89351473922902491</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D13">
+        <v>-84</v>
+      </c>
+      <c r="E13" s="3">
+        <f>E12-1</f>
+        <v>39406</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89356009070294784</v>
+      </c>
+      <c r="G13">
+        <v>-86</v>
+      </c>
+      <c r="H13" s="4">
+        <v>39402</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.8934693877551021</v>
+      </c>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D14">
+        <v>-84</v>
+      </c>
+      <c r="E14" s="3">
+        <f>E13+2</f>
+        <v>39408</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89360544217687077</v>
+      </c>
+      <c r="G14">
+        <v>-87</v>
+      </c>
+      <c r="H14" s="4">
+        <v>39404</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89351473922902491</v>
+      </c>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D15">
+        <v>-85</v>
+      </c>
+      <c r="E15" s="3">
+        <f>E14+2</f>
+        <v>39410</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8936507936507937</v>
+      </c>
+      <c r="G15">
+        <v>-88</v>
+      </c>
+      <c r="H15" s="4">
+        <v>39406</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89356009070294784</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D16">
+        <v>-85</v>
+      </c>
+      <c r="E16" s="3">
+        <f>E15-2</f>
+        <v>39408</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89360544217687077</v>
+      </c>
+      <c r="G16">
+        <v>-87</v>
+      </c>
+      <c r="H16" s="4">
+        <v>39404</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89351473922902491</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D17">
+        <v>-86</v>
+      </c>
+      <c r="E17" s="3">
+        <f>E16-2</f>
+        <v>39406</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89356009070294784</v>
+      </c>
+      <c r="G17">
+        <v>-86</v>
+      </c>
+      <c r="H17" s="4">
+        <v>39406</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89356009070294784</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D18">
+        <v>-86</v>
+      </c>
+      <c r="E18" s="3">
+        <f>E17+2</f>
+        <v>39408</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89360544217687077</v>
+      </c>
+      <c r="G18">
+        <v>-87</v>
+      </c>
+      <c r="H18" s="4">
+        <v>39406</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89356009070294784</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D19">
+        <v>-86</v>
+      </c>
+      <c r="E19" s="3">
+        <f>E18-2</f>
+        <v>39406</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89356009070294784</v>
+      </c>
+      <c r="G19">
+        <v>-78</v>
+      </c>
+      <c r="H19" s="4">
+        <v>39404</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89351473922902491</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D20">
+        <v>-82</v>
+      </c>
+      <c r="E20" s="3">
+        <f>E19-4</f>
+        <v>39402</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8934693877551021</v>
+      </c>
+      <c r="G20">
+        <v>-84</v>
+      </c>
+      <c r="H20" s="4">
+        <v>39398</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89337868480725624</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D21">
+        <v>-89</v>
+      </c>
+      <c r="E21" s="3">
+        <f>E20+11</f>
+        <v>39413</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89371882086167798</v>
+      </c>
+      <c r="G21">
+        <v>-92</v>
+      </c>
+      <c r="H21" s="4">
+        <v>39411</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89367346938775505</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D22">
+        <v>-89</v>
+      </c>
+      <c r="E22" s="3">
+        <f>E21+1</f>
+        <v>39414</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89374149659863944</v>
+      </c>
+      <c r="G22">
+        <v>-90</v>
+      </c>
+      <c r="H22" s="4">
+        <v>39411</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89367346938775505</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D23">
+        <v>-89</v>
+      </c>
+      <c r="E23" s="3">
+        <f>E22</f>
+        <v>39414</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89374149659863944</v>
+      </c>
+      <c r="G23">
+        <v>-90</v>
+      </c>
+      <c r="H23" s="4">
+        <v>39413</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89371882086167798</v>
+      </c>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D24">
+        <v>-90</v>
+      </c>
+      <c r="E24" s="3">
+        <f>E23+4</f>
+        <v>39418</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8938321995464853</v>
+      </c>
+      <c r="G24">
+        <v>-92</v>
+      </c>
+      <c r="H24" s="4">
+        <v>39414</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89374149659863944</v>
+      </c>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D25">
+        <v>-93</v>
+      </c>
+      <c r="E25" s="3">
+        <f>E24</f>
+        <v>39418</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8938321995464853</v>
+      </c>
+      <c r="G25">
+        <v>-93</v>
+      </c>
+      <c r="H25" s="4">
+        <v>39418</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="1"/>
+        <v>0.8938321995464853</v>
+      </c>
+    </row>
+    <row r="26" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D26">
+        <v>-92</v>
+      </c>
+      <c r="E26" s="3">
+        <f>E25-1</f>
+        <v>39417</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89380952380952383</v>
+      </c>
+      <c r="G26">
+        <v>-92</v>
+      </c>
+      <c r="H26" s="4">
+        <v>39416</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89378684807256237</v>
+      </c>
+    </row>
+    <row r="27" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D27">
+        <v>-92</v>
+      </c>
+      <c r="E27" s="3">
+        <f>E26</f>
+        <v>39417</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89380952380952383</v>
+      </c>
+      <c r="G27">
+        <v>-93</v>
+      </c>
+      <c r="H27" s="4">
+        <v>39416</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89378684807256237</v>
+      </c>
+    </row>
+    <row r="28" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D28">
+        <v>-92</v>
+      </c>
+      <c r="E28" s="3">
+        <f>E27</f>
+        <v>39417</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89380952380952383</v>
+      </c>
+      <c r="G28">
+        <v>-92</v>
+      </c>
+      <c r="H28" s="4">
+        <f>H27</f>
+        <v>39416</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89378684807256237</v>
+      </c>
+    </row>
+    <row r="29" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D29">
+        <v>-92</v>
+      </c>
+      <c r="E29" s="3">
+        <f>E28+3</f>
+        <v>39420</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89387755102040811</v>
+      </c>
+      <c r="G29">
+        <v>-93</v>
+      </c>
+      <c r="H29" s="4">
+        <v>39418</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="1"/>
+        <v>0.8938321995464853</v>
+      </c>
+    </row>
+    <row r="30" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D30">
+        <v>-92</v>
+      </c>
+      <c r="E30" s="3">
+        <f>E29-2</f>
+        <v>39418</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8938321995464853</v>
+      </c>
+      <c r="G30">
+        <v>-93</v>
+      </c>
+      <c r="H30" s="4">
+        <v>39418</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="1"/>
+        <v>0.8938321995464853</v>
+      </c>
+    </row>
+    <row r="31" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D31">
+        <v>-92</v>
+      </c>
+      <c r="E31" s="3">
+        <f>E30-2</f>
+        <v>39416</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89378684807256237</v>
+      </c>
+      <c r="G31">
+        <v>-91</v>
+      </c>
+      <c r="H31" s="4">
+        <v>39418</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="1"/>
+        <v>0.8938321995464853</v>
+      </c>
+    </row>
+    <row r="32" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D32">
+        <v>-92</v>
+      </c>
+      <c r="E32" s="3">
+        <f>E31+2</f>
+        <v>39418</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8938321995464853</v>
+      </c>
+      <c r="G32">
+        <v>-92</v>
+      </c>
+      <c r="H32" s="4">
+        <v>39420</v>
+      </c>
+      <c r="I32" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89387755102040811</v>
+      </c>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D33">
+        <v>-93</v>
+      </c>
+      <c r="E33" s="3">
+        <f>E32+3</f>
+        <v>39421</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89390022675736958</v>
+      </c>
+      <c r="G33">
+        <v>-94</v>
+      </c>
+      <c r="H33" s="4">
+        <v>39419</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89385487528344676</v>
+      </c>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D34">
+        <v>-93</v>
+      </c>
+      <c r="E34" s="3">
+        <f>E33</f>
+        <v>39421</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89390022675736958</v>
+      </c>
+      <c r="G34">
+        <v>-93</v>
+      </c>
+      <c r="H34" s="4">
+        <v>39419</v>
+      </c>
+      <c r="I34" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89385487528344676</v>
+      </c>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D35">
+        <v>-93</v>
+      </c>
+      <c r="E35" s="3">
+        <f>E34-1</f>
+        <v>39420</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89387755102040811</v>
+      </c>
+      <c r="G35">
+        <v>-94</v>
+      </c>
+      <c r="H35" s="4">
+        <v>39419</v>
+      </c>
+      <c r="I35" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89385487528344676</v>
+      </c>
+    </row>
+    <row r="36" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D36">
+        <v>-93</v>
+      </c>
+      <c r="E36" s="3">
+        <f>E35</f>
+        <v>39420</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89387755102040811</v>
+      </c>
+      <c r="G36">
+        <v>-94</v>
+      </c>
+      <c r="H36" s="4">
+        <v>39419</v>
+      </c>
+      <c r="I36" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89385487528344676</v>
+      </c>
+    </row>
+    <row r="37" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D37">
+        <v>-93</v>
+      </c>
+      <c r="E37" s="3">
+        <f>E36</f>
+        <v>39420</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89387755102040811</v>
+      </c>
+      <c r="G37">
+        <v>-93</v>
+      </c>
+      <c r="H37" s="4">
+        <v>39419</v>
+      </c>
+      <c r="I37" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89385487528344676</v>
+      </c>
+    </row>
+    <row r="38" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D38">
+        <v>-94</v>
+      </c>
+      <c r="E38" s="6">
+        <f>E37</f>
+        <v>39420</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89387755102040811</v>
+      </c>
+      <c r="G38">
+        <v>-94</v>
+      </c>
+      <c r="H38" s="3">
+        <v>39419</v>
+      </c>
+      <c r="I38" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89385487528344676</v>
+      </c>
+    </row>
+    <row r="39" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D39">
+        <v>-93</v>
+      </c>
+      <c r="E39" s="6">
+        <f>E38-1</f>
+        <v>39419</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89385487528344676</v>
+      </c>
+      <c r="G39">
+        <v>-93</v>
+      </c>
+      <c r="H39" s="3">
+        <v>39420</v>
+      </c>
+      <c r="I39" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89387755102040811</v>
+      </c>
+    </row>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D40">
+        <v>-94</v>
+      </c>
+      <c r="E40" s="6">
+        <f>E39</f>
+        <v>39419</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89385487528344676</v>
+      </c>
+      <c r="G40">
+        <v>-93</v>
+      </c>
+      <c r="H40" s="3">
+        <v>39421</v>
+      </c>
+      <c r="I40" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89390022675736958</v>
+      </c>
+    </row>
+    <row r="41" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D41">
+        <v>-95</v>
+      </c>
+      <c r="E41" s="6">
+        <f>E40+3</f>
+        <v>39422</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89392290249433104</v>
+      </c>
+      <c r="G41">
+        <v>-95</v>
+      </c>
+      <c r="H41" s="3">
+        <v>39422</v>
+      </c>
+      <c r="I41" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89392290249433104</v>
+      </c>
+    </row>
+    <row r="42" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D42">
+        <v>-94</v>
+      </c>
+      <c r="E42" s="6">
+        <f>E41</f>
+        <v>39422</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89392290249433104</v>
+      </c>
+      <c r="G42">
+        <v>-94</v>
+      </c>
+      <c r="H42" s="3">
+        <v>39424</v>
+      </c>
+      <c r="I42" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89396825396825397</v>
+      </c>
+    </row>
+    <row r="43" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D43">
+        <v>-95</v>
+      </c>
+      <c r="E43" s="6">
+        <f>E42</f>
+        <v>39422</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89392290249433104</v>
+      </c>
+      <c r="G43">
+        <v>-95</v>
+      </c>
+      <c r="H43" s="3">
+        <v>39422</v>
+      </c>
+      <c r="I43" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89392290249433104</v>
+      </c>
+    </row>
+    <row r="44" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D44">
+        <v>-95</v>
+      </c>
+      <c r="E44" s="6">
+        <f>E43</f>
+        <v>39422</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89392290249433104</v>
+      </c>
+      <c r="G44">
+        <v>-94</v>
+      </c>
+      <c r="H44" s="3">
+        <f>H43</f>
+        <v>39422</v>
+      </c>
+      <c r="I44" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89392290249433104</v>
+      </c>
+    </row>
+    <row r="45" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D45">
+        <v>-96</v>
+      </c>
+      <c r="E45" s="6">
+        <f>E44+2</f>
+        <v>39424</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89396825396825397</v>
+      </c>
+      <c r="G45">
+        <v>-96</v>
+      </c>
+      <c r="H45" s="3">
+        <v>39424</v>
+      </c>
+      <c r="I45" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89396825396825397</v>
+      </c>
+    </row>
+    <row r="46" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D46">
+        <v>-95</v>
+      </c>
+      <c r="E46" s="6">
+        <f>E45-4</f>
+        <v>39420</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89387755102040811</v>
+      </c>
+      <c r="G46">
+        <v>-94</v>
+      </c>
+      <c r="H46" s="3">
+        <v>39424</v>
+      </c>
+      <c r="I46" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89396825396825397</v>
+      </c>
+    </row>
+    <row r="47" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D47">
+        <v>-95</v>
+      </c>
+      <c r="E47" s="6">
+        <f>E46+2</f>
+        <v>39422</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89392290249433104</v>
+      </c>
+      <c r="G47">
+        <v>-95</v>
+      </c>
+      <c r="H47" s="3">
+        <v>39424</v>
+      </c>
+      <c r="I47" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89396825396825397</v>
+      </c>
+    </row>
+    <row r="48" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D48">
+        <v>-96</v>
+      </c>
+      <c r="E48" s="6">
+        <f>E47+2</f>
+        <v>39424</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89396825396825397</v>
+      </c>
+      <c r="G48">
+        <v>-96</v>
+      </c>
+      <c r="H48" s="3">
+        <v>39426</v>
+      </c>
+      <c r="I48" s="1">
+        <f t="shared" si="1"/>
+        <v>0.8940136054421769</v>
+      </c>
+    </row>
+    <row r="49" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D49">
+        <v>-96</v>
+      </c>
+      <c r="E49" s="6">
+        <f>E48</f>
+        <v>39424</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89396825396825397</v>
+      </c>
+      <c r="G49">
+        <v>-95</v>
+      </c>
+      <c r="H49" s="3">
+        <v>39426</v>
+      </c>
+      <c r="I49" s="1">
+        <f t="shared" si="1"/>
+        <v>0.8940136054421769</v>
+      </c>
+    </row>
+    <row r="50" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D50">
+        <v>-96</v>
+      </c>
+      <c r="E50" s="6">
+        <f>E49+1</f>
+        <v>39425</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89399092970521543</v>
+      </c>
+      <c r="G50">
+        <v>-96</v>
+      </c>
+      <c r="H50" s="3">
+        <v>39427</v>
+      </c>
+      <c r="I50" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89403628117913836</v>
+      </c>
+    </row>
+    <row r="51" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D51">
+        <v>-97</v>
+      </c>
+      <c r="E51" s="6">
+        <f>E50+1</f>
+        <v>39426</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8940136054421769</v>
+      </c>
+      <c r="G51">
+        <v>-97</v>
+      </c>
+      <c r="H51" s="3">
+        <v>39427</v>
+      </c>
+      <c r="I51" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89403628117913836</v>
+      </c>
+    </row>
+    <row r="52" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D52">
+        <v>-97</v>
+      </c>
+      <c r="E52" s="6">
+        <f>E51</f>
+        <v>39426</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8940136054421769</v>
+      </c>
+      <c r="G52">
+        <v>-97</v>
+      </c>
+      <c r="H52" s="3">
+        <v>39428</v>
+      </c>
+      <c r="I52" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89405895691609982</v>
+      </c>
+    </row>
+    <row r="53" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D53">
+        <v>-97</v>
+      </c>
+      <c r="E53" s="6">
+        <f>E52</f>
+        <v>39426</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8940136054421769</v>
+      </c>
+      <c r="G53">
+        <v>-97</v>
+      </c>
+      <c r="H53" s="3">
+        <v>39427</v>
+      </c>
+      <c r="I53" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89403628117913836</v>
+      </c>
+    </row>
+    <row r="54" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D54">
+        <v>-97</v>
+      </c>
+      <c r="E54" s="6">
+        <f>E53+1</f>
+        <v>39427</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89403628117913836</v>
+      </c>
+      <c r="G54">
+        <v>-97</v>
+      </c>
+      <c r="H54" s="3">
+        <v>39428</v>
+      </c>
+      <c r="I54" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89405895691609982</v>
+      </c>
+    </row>
+    <row r="55" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D55">
+        <v>-98</v>
+      </c>
+      <c r="E55" s="6">
+        <f>E54</f>
+        <v>39427</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89403628117913836</v>
+      </c>
+      <c r="G55">
+        <v>-97</v>
+      </c>
+      <c r="H55" s="3">
+        <f>H54</f>
+        <v>39428</v>
+      </c>
+      <c r="I55" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89405895691609982</v>
+      </c>
+    </row>
+    <row r="56" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D56">
+        <v>-99</v>
+      </c>
+      <c r="E56" s="6">
+        <f>E55+3</f>
+        <v>39430</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89410430839002264</v>
+      </c>
+      <c r="G56">
+        <v>-99</v>
+      </c>
+      <c r="H56" s="3">
+        <v>39431</v>
+      </c>
+      <c r="I56" s="1">
+        <f t="shared" si="1"/>
+        <v>0.8941269841269841</v>
+      </c>
+    </row>
+    <row r="57" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D57">
+        <v>-99</v>
+      </c>
+      <c r="E57" s="6">
+        <f>E56</f>
+        <v>39430</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89410430839002264</v>
+      </c>
+      <c r="G57">
+        <v>-99</v>
+      </c>
+      <c r="H57" s="3">
+        <v>39431</v>
+      </c>
+      <c r="I57" s="1">
+        <f t="shared" si="1"/>
+        <v>0.8941269841269841</v>
+      </c>
+    </row>
+    <row r="58" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D58">
+        <v>-99</v>
+      </c>
+      <c r="E58" s="6">
+        <f>E57-1</f>
+        <v>39429</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89408163265306118</v>
+      </c>
+      <c r="G58">
+        <v>-98</v>
+      </c>
+      <c r="H58" s="3">
+        <v>39432</v>
+      </c>
+      <c r="I58" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89414965986394557</v>
+      </c>
+    </row>
+    <row r="59" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D59">
+        <v>-100</v>
+      </c>
+      <c r="E59" s="6">
+        <f>E58+1</f>
+        <v>39430</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89410430839002264</v>
+      </c>
+      <c r="G59">
+        <v>-99</v>
+      </c>
+      <c r="H59" s="3">
+        <v>39432</v>
+      </c>
+      <c r="I59" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89414965986394557</v>
+      </c>
+    </row>
+    <row r="60" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D60">
+        <v>-99</v>
+      </c>
+      <c r="E60" s="6">
+        <f>E59</f>
+        <v>39430</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89410430839002264</v>
+      </c>
+      <c r="G60">
+        <v>-98</v>
+      </c>
+      <c r="H60" s="3">
+        <v>39432</v>
+      </c>
+      <c r="I60" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89414965986394557</v>
+      </c>
+    </row>
+    <row r="61" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D61">
+        <v>-99</v>
+      </c>
+      <c r="E61" s="7">
+        <f>E60+1</f>
+        <v>39431</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8941269841269841</v>
+      </c>
+      <c r="G61">
+        <v>-99</v>
+      </c>
+      <c r="H61" s="3">
+        <v>39432</v>
+      </c>
+      <c r="I61" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89414965986394557</v>
+      </c>
+    </row>
+    <row r="62" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D62">
+        <v>-100</v>
+      </c>
+      <c r="E62" s="7">
+        <f>E61+1</f>
+        <v>39432</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89414965986394557</v>
+      </c>
+      <c r="G62">
+        <v>-100</v>
+      </c>
+      <c r="H62" s="3">
+        <v>39432</v>
+      </c>
+      <c r="I62" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89414965986394557</v>
+      </c>
+    </row>
+    <row r="63" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D63">
+        <v>-100</v>
+      </c>
+      <c r="E63" s="7">
+        <f>E62-1</f>
+        <v>39431</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8941269841269841</v>
+      </c>
+      <c r="G63">
+        <v>-99</v>
+      </c>
+      <c r="H63" s="3">
+        <v>39433</v>
+      </c>
+      <c r="I63" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89417233560090703</v>
+      </c>
+    </row>
+    <row r="64" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D64">
+        <v>-100</v>
+      </c>
+      <c r="E64" s="7">
+        <f>E63</f>
+        <v>39431</v>
+      </c>
+      <c r="F64" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8941269841269841</v>
+      </c>
+      <c r="G64">
+        <v>-99</v>
+      </c>
+      <c r="H64" s="3">
+        <v>39433</v>
+      </c>
+      <c r="I64" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89417233560090703</v>
+      </c>
+    </row>
+    <row r="65" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D65">
+        <v>-100</v>
+      </c>
+      <c r="E65" s="7">
+        <f>E64</f>
+        <v>39431</v>
+      </c>
+      <c r="F65" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8941269841269841</v>
+      </c>
+      <c r="G65">
+        <v>-99</v>
+      </c>
+      <c r="H65" s="3">
+        <v>39434</v>
+      </c>
+      <c r="I65" s="1">
+        <f t="shared" si="1"/>
+        <v>0.8941950113378685</v>
+      </c>
+    </row>
+    <row r="66" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D66">
+        <v>-101</v>
+      </c>
+      <c r="E66" s="7">
+        <f>E65+1</f>
+        <v>39432</v>
+      </c>
+      <c r="F66" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89414965986394557</v>
+      </c>
+      <c r="G66">
+        <v>-100</v>
+      </c>
+      <c r="H66" s="3">
+        <v>39434</v>
+      </c>
+      <c r="I66" s="1">
+        <f t="shared" si="1"/>
+        <v>0.8941950113378685</v>
+      </c>
+    </row>
+    <row r="67" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D67">
+        <v>-101</v>
+      </c>
+      <c r="E67" s="7">
+        <f>E66+1</f>
+        <v>39433</v>
+      </c>
+      <c r="F67" s="1">
+        <f t="shared" ref="F67:F79" si="2">E67/44100</f>
+        <v>0.89417233560090703</v>
+      </c>
+      <c r="G67">
+        <v>-101</v>
+      </c>
+      <c r="H67" s="3">
+        <v>39435</v>
+      </c>
+      <c r="I67" s="1">
+        <f t="shared" ref="I67:I79" si="3">H67/44100</f>
+        <v>0.89421768707482996</v>
+      </c>
+    </row>
+    <row r="68" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D68">
+        <v>-101</v>
+      </c>
+      <c r="E68" s="7">
+        <f>E67+1</f>
+        <v>39434</v>
+      </c>
+      <c r="F68" s="1">
+        <f t="shared" si="2"/>
+        <v>0.8941950113378685</v>
+      </c>
+      <c r="G68">
+        <v>-101</v>
+      </c>
+      <c r="H68" s="3">
+        <v>39437</v>
+      </c>
+      <c r="I68" s="1">
+        <f t="shared" si="3"/>
+        <v>0.89426303854875289</v>
+      </c>
+    </row>
+    <row r="69" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D69">
+        <v>-102</v>
+      </c>
+      <c r="E69" s="7">
+        <f>E68+2</f>
+        <v>39436</v>
+      </c>
+      <c r="F69" s="1">
+        <f t="shared" si="2"/>
+        <v>0.89424036281179142</v>
+      </c>
+      <c r="G69">
+        <v>-102</v>
+      </c>
+      <c r="H69" s="3">
+        <v>39437</v>
+      </c>
+      <c r="I69" s="1">
+        <f t="shared" si="3"/>
+        <v>0.89426303854875289</v>
+      </c>
+    </row>
+    <row r="70" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D70">
+        <v>-102</v>
+      </c>
+      <c r="E70" s="7">
+        <f>E69</f>
+        <v>39436</v>
+      </c>
+      <c r="F70" s="1">
+        <f t="shared" si="2"/>
+        <v>0.89424036281179142</v>
+      </c>
+      <c r="G70">
+        <v>-102</v>
+      </c>
+      <c r="H70" s="3">
+        <v>39437</v>
+      </c>
+      <c r="I70" s="1">
+        <f t="shared" si="3"/>
+        <v>0.89426303854875289</v>
+      </c>
+    </row>
+    <row r="71" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D71">
+        <v>-102</v>
+      </c>
+      <c r="E71" s="7">
+        <f>E70+1</f>
+        <v>39437</v>
+      </c>
+      <c r="F71" s="1">
+        <f t="shared" si="2"/>
+        <v>0.89426303854875289</v>
+      </c>
+      <c r="G71">
+        <v>-102</v>
+      </c>
+      <c r="H71" s="3">
+        <v>39439</v>
+      </c>
+      <c r="I71" s="1">
+        <f t="shared" si="3"/>
+        <v>0.8943083900226757</v>
+      </c>
+    </row>
+    <row r="72" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D72">
+        <v>-103</v>
+      </c>
+      <c r="E72" s="7">
+        <f>E71+2</f>
+        <v>39439</v>
+      </c>
+      <c r="F72" s="1">
+        <f t="shared" si="2"/>
+        <v>0.8943083900226757</v>
+      </c>
+      <c r="G72">
+        <v>-104</v>
+      </c>
+      <c r="H72" s="3">
+        <v>39440</v>
+      </c>
+      <c r="I72" s="1">
+        <f t="shared" si="3"/>
+        <v>0.89433106575963717</v>
+      </c>
+    </row>
+    <row r="73" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D73">
+        <v>-104</v>
+      </c>
+      <c r="E73" s="7">
+        <f>E72</f>
+        <v>39439</v>
+      </c>
+      <c r="F73" s="1">
+        <f t="shared" si="2"/>
+        <v>0.8943083900226757</v>
+      </c>
+      <c r="G73">
+        <v>-104</v>
+      </c>
+      <c r="H73" s="3">
+        <v>39440</v>
+      </c>
+      <c r="I73" s="1">
+        <f t="shared" si="3"/>
+        <v>0.89433106575963717</v>
+      </c>
+    </row>
+    <row r="74" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D74">
+        <v>-104</v>
+      </c>
+      <c r="E74" s="7">
+        <f>E73</f>
+        <v>39439</v>
+      </c>
+      <c r="F74" s="1">
+        <f t="shared" si="2"/>
+        <v>0.8943083900226757</v>
+      </c>
+      <c r="G74">
+        <v>-103</v>
+      </c>
+      <c r="H74" s="3">
+        <v>39440</v>
+      </c>
+      <c r="I74" s="1">
+        <f t="shared" si="3"/>
+        <v>0.89433106575963717</v>
+      </c>
+    </row>
+    <row r="75" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D75">
+        <v>-103</v>
+      </c>
+      <c r="E75" s="7">
+        <f>E74+1</f>
+        <v>39440</v>
+      </c>
+      <c r="F75" s="1">
+        <f t="shared" si="2"/>
+        <v>0.89433106575963717</v>
+      </c>
+      <c r="G75">
+        <v>-104</v>
+      </c>
+      <c r="H75" s="3">
+        <v>39441</v>
+      </c>
+      <c r="I75" s="1">
+        <f t="shared" si="3"/>
+        <v>0.89435374149659863</v>
+      </c>
+    </row>
+    <row r="76" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D76">
+        <v>-106</v>
+      </c>
+      <c r="E76" s="7">
+        <f>E75+2</f>
+        <v>39442</v>
+      </c>
+      <c r="F76" s="1">
+        <f t="shared" si="2"/>
+        <v>0.89437641723356009</v>
+      </c>
+      <c r="G76">
+        <v>-105</v>
+      </c>
+      <c r="H76" s="3">
+        <v>39442</v>
+      </c>
+      <c r="I76" s="1">
+        <f t="shared" si="3"/>
+        <v>0.89437641723356009</v>
+      </c>
+    </row>
+    <row r="77" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D77">
+        <v>-106</v>
+      </c>
+      <c r="E77" s="7">
+        <f>E76+2</f>
+        <v>39444</v>
+      </c>
+      <c r="F77" s="1">
+        <f t="shared" si="2"/>
+        <v>0.89442176870748302</v>
+      </c>
+      <c r="G77">
+        <v>-106</v>
+      </c>
+      <c r="H77" s="3">
+        <v>39443</v>
+      </c>
+      <c r="I77" s="1">
+        <f t="shared" si="3"/>
+        <v>0.89439909297052156</v>
+      </c>
+    </row>
+    <row r="78" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D78">
+        <v>-105</v>
+      </c>
+      <c r="E78" s="7">
+        <f>E77</f>
+        <v>39444</v>
+      </c>
+      <c r="F78" s="1">
+        <f t="shared" si="2"/>
+        <v>0.89442176870748302</v>
+      </c>
+      <c r="G78">
+        <v>-106</v>
+      </c>
+      <c r="H78" s="3">
+        <v>39443</v>
+      </c>
+      <c r="I78" s="1">
+        <f t="shared" si="3"/>
+        <v>0.89439909297052156</v>
+      </c>
+    </row>
+    <row r="79" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D79">
+        <v>-105</v>
+      </c>
+      <c r="E79" s="7">
+        <f>E78</f>
+        <v>39444</v>
+      </c>
+      <c r="F79" s="1">
+        <f t="shared" si="2"/>
+        <v>0.89442176870748302</v>
+      </c>
+      <c r="G79">
+        <v>-106</v>
+      </c>
+      <c r="H79" s="3">
+        <v>39443</v>
+      </c>
+      <c r="I79" s="1">
+        <f t="shared" si="3"/>
+        <v>0.89439909297052156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>